<commit_message>
A lot of updates
</commit_message>
<xml_diff>
--- a/public/data/events.xlsx
+++ b/public/data/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Codes\Recis React\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5B78E5-BD40-4E93-8317-AE49E369E325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC4C44E-8F46-4E76-A0ED-D219F1729450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="3075" windowWidth="20385" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>/Pensi</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>Now</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,21 +448,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -459,12 +471,12 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -473,12 +485,12 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -487,29 +499,29 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -520,15 +532,29 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>